<commit_message>
add b5 b6 b7
</commit_message>
<xml_diff>
--- a/elfelf2/evidence.xlsx
+++ b/elfelf2/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caner\Desktop\testnets\game-of-nfts\elf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BDA616-3FCB-45F8-87FD-FF788766A95B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB496AB7-0CB8-4B96-B185-2E70C6453519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="13" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -317,6 +312,24 @@
   </si>
   <si>
     <t>B5D8EC25EBCD83A8BB2AD95C60F32BB4E1E04707EE1359955D08C91D1F99DA2C</t>
+  </si>
+  <si>
+    <t>491D20AFDEFE6A383249BF1551D080FCF1FE7ED207541BCB9ED4DC7199B8C0F9</t>
+  </si>
+  <si>
+    <t>73ABDAA5F7620413FE46EFB005051D7E46FEF9C2A090684349C52AD9B4EDA369</t>
+  </si>
+  <si>
+    <t>6D6653C42C29E7144665F8BE03B9CEBF96B3B965E37A22FFF4339B04A9E34949</t>
+  </si>
+  <si>
+    <t>289C0AFF2ADCA5172A2E9849ECCFFEA2120D599428F3BAD5BB61C1DB34F2370F</t>
+  </si>
+  <si>
+    <t>3147ACC180D0FF0177E1D5EF92097EA73FACEB3C7A78E57D73ABEC92605C868B</t>
+  </si>
+  <si>
+    <t>B5C96EFF4BE634B84DC9FA1551BBE6E1AE521C0DAAD044A2622D56A46D3A45C7</t>
   </si>
 </sst>
 </file>
@@ -729,54 +742,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" t="s">
         <v>19</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -803,18 +816,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -841,18 +854,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -879,10 +892,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -898,15 +949,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,34 +968,58 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,48 +1033,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1020,48 +1095,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1082,48 +1157,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1144,48 +1219,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1206,55 +1281,92 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,92 +1380,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,133 +1458,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1523,6 +1536,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1537,15 +1586,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,14 +1622,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1594,46 +1645,42 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C30B6F-210C-4EF1-92E0-F564E13FCE9A}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1663,32 +1710,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1719,27 +1766,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1770,27 +1817,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1821,27 +1868,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1873,27 +1920,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1920,10 +1967,48 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1937,42 +2022,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>